<commit_message>
update building, dah, balkonu
update building, dah, balkonu
</commit_message>
<xml_diff>
--- a/балкон/вартість_балконів_стяжки.xlsx
+++ b/балкон/вартість_балконів_стяжки.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20730" windowHeight="10050" tabRatio="830" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20730" windowHeight="10050" tabRatio="830" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="підїзд1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="284">
   <si>
     <t>підїзд</t>
   </si>
@@ -1247,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1905,6 +1905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2209,7 +2210,7 @@
   <dimension ref="A1:S76"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5211,7 +5212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -12145,7 +12146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -15497,7 +15498,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:J10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15638,10 +15639,12 @@
         <f>G5*'розрахунок квадрату стяжки'!$M$3</f>
         <v>15737.894647342713</v>
       </c>
-      <c r="I5" s="88"/>
+      <c r="I5" s="88">
+        <v>16000</v>
+      </c>
       <c r="J5" s="77">
         <f t="shared" si="1"/>
-        <v>-15737.894647342713</v>
+        <v>262.10535265728686</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -15792,9 +15795,13 @@
         <f>SUM(H2:H10)</f>
         <v>40457.137074161634</v>
       </c>
+      <c r="I11">
+        <f>SUM(I2:I10)</f>
+        <v>16000</v>
+      </c>
       <c r="J11">
         <f>SUM(J2:J10)</f>
-        <v>-40457.137074161634</v>
+        <v>-24457.137074161637</v>
       </c>
     </row>
   </sheetData>
@@ -16706,10 +16713,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D10"/>
+  <dimension ref="A3:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16717,127 +16724,166 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="77"/>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="267" t="s">
         <v>228</v>
       </c>
       <c r="C3" s="77" t="s">
         <v>265</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="77" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="77">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="267" t="s">
         <v>229</v>
       </c>
       <c r="C4" s="121">
         <f>підїзд1!P48</f>
         <v>161607.76170527149</v>
       </c>
-      <c r="D4" s="119">
+      <c r="D4" s="121">
         <f>підїзд1!Q48</f>
         <v>70044</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="121">
+        <f>D4-C4</f>
+        <v>-91563.761705271492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="77">
         <v>2</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="267" t="s">
         <v>230</v>
       </c>
       <c r="C5" s="121">
         <f>підїзд2!P39</f>
         <v>164749.35895142169</v>
       </c>
-      <c r="D5" s="119">
+      <c r="D5" s="121">
         <f>підїзд2!Q39</f>
         <v>84690</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="121">
+        <f t="shared" ref="E5:E10" si="0">D5-C5</f>
+        <v>-80059.358951421687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="78">
         <v>3</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="267" t="s">
         <v>231</v>
       </c>
       <c r="C6" s="165">
         <f>підїзд3!P48</f>
         <v>134748.14664981136</v>
       </c>
-      <c r="D6" s="119">
+      <c r="D6" s="121">
         <f>підїзд3!Q48</f>
         <v>51042</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="121">
+        <f t="shared" si="0"/>
+        <v>-83706.146649811359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="78">
         <v>4</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="267" t="s">
         <v>232</v>
       </c>
       <c r="C7" s="121">
         <f>підїзд4!P30</f>
         <v>84778.189693441818</v>
       </c>
-      <c r="D7" s="119">
+      <c r="D7" s="121">
         <f>підїзд4!Q30</f>
         <v>37977</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="121">
+        <f t="shared" si="0"/>
+        <v>-46801.189693441818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="78">
         <v>5</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="267" t="s">
         <v>233</v>
       </c>
       <c r="C8" s="121">
         <f>підїзд5!P57</f>
         <v>169246.86396428419</v>
       </c>
-      <c r="D8" s="119">
+      <c r="D8" s="121">
         <f>підїзд5!Q57</f>
         <v>83996</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="121">
+        <f t="shared" si="0"/>
+        <v>-85250.863964284188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="77">
         <v>6</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="267" t="s">
         <v>271</v>
       </c>
       <c r="C9" s="77">
         <f>комерція!H11</f>
         <v>40457.137074161634</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="77">
         <f>комерція!I11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="119">
+        <v>16000</v>
+      </c>
+      <c r="E9" s="121">
+        <f t="shared" si="0"/>
+        <v>-24457.137074161634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="250" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="252"/>
+      <c r="C10" s="121">
         <f>SUM(C4:C9)</f>
         <v>755587.45803839224</v>
       </c>
-      <c r="D10" s="119">
+      <c r="D10" s="121">
         <f>SUM(D4:D9)</f>
-        <v>327749</v>
+        <v>343749</v>
+      </c>
+      <c r="E10" s="121">
+        <f t="shared" si="0"/>
+        <v>-411838.45803839224</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>